<commit_message>
Added reporting period ID to documents API
</commit_message>
<xml_diff>
--- a/tests/server/fixtures/file-success/GOV-075-09302020-simple-v1.xlsx
+++ b/tests/server/fixtures/file-success/GOV-075-09302020-simple-v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/usdr/cares-reporter/tests/server/fixtures/file-success/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEC7A24-5132-6045-90CA-D5F6BB4EB882}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602A993A-A1EE-5845-9605-3067567008B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="45780" windowHeight="8420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Certification" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="345">
   <si>
     <t>Certification</t>
   </si>
@@ -543,9 +543,6 @@
   </si>
   <si>
     <t>Other</t>
-  </si>
-  <si>
-    <t>3674861</t>
   </si>
   <si>
     <t>Award Number</t>
@@ -7897,36 +7894,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="37.5" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>132</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1">
       <c r="A2" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B3" s="17">
         <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" s="46">
         <v>2163121.9700000002</v>
@@ -7937,13 +7934,13 @@
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="17">
         <v>75</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D4" s="46">
         <v>5957909</v>
@@ -7954,13 +7951,13 @@
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1">
       <c r="A6" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B6" s="17"/>
     </row>
@@ -8983,13 +8980,13 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>132</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1">
@@ -8997,7 +8994,7 @@
         <v>75</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="41">
         <v>1567999.5</v>
@@ -10028,46 +10025,46 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
       <c r="A1" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="C1" s="47" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="D1" s="47" t="s">
         <v>220</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="E1" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>220</v>
+      </c>
+      <c r="H1" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="E1" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="F1" s="47" t="s">
+      <c r="I1" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="47" t="s">
-        <v>221</v>
-      </c>
-      <c r="H1" s="47" t="s">
+      <c r="J1" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="L1" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="I1" s="47" t="s">
-        <v>212</v>
-      </c>
-      <c r="J1" s="47" t="s">
-        <v>212</v>
-      </c>
-      <c r="K1" s="47" t="s">
-        <v>214</v>
-      </c>
-      <c r="L1" s="47" t="s">
+      <c r="M1" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="N1" s="47" t="s">
         <v>223</v>
-      </c>
-      <c r="M1" s="47" t="s">
-        <v>223</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>224</v>
       </c>
       <c r="O1" s="47"/>
       <c r="P1" s="47"/>
@@ -10084,7 +10081,7 @@
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>7</v>
@@ -10096,34 +10093,34 @@
         <v>39</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F2" s="48" t="s">
         <v>117</v>
       </c>
       <c r="G2" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="H2" s="48" t="s">
         <v>227</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="I2" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="I2" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="J2" s="48" t="s">
-        <v>229</v>
-      </c>
       <c r="K2" s="48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L2" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="M2" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="M2" s="48" t="s">
-        <v>209</v>
-      </c>
       <c r="N2" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O2" s="47"/>
       <c r="P2" s="47"/>
@@ -10140,149 +10137,149 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
       <c r="A3" s="47" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>233</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>234</v>
       </c>
       <c r="G3" s="17">
         <v>1</v>
       </c>
       <c r="H3" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="I3" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="I3" s="17" t="s">
-        <v>236</v>
-      </c>
       <c r="J3" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M3" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N3" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1">
       <c r="B4" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>239</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>240</v>
       </c>
       <c r="G4" s="17">
         <v>2</v>
       </c>
       <c r="H4" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="J4" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="J4" s="17" t="s">
+      <c r="K4" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="K4" s="17" t="s">
-        <v>243</v>
-      </c>
       <c r="L4" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="B5" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="49" t="s">
         <v>247</v>
       </c>
-      <c r="G5" s="49" t="s">
-        <v>248</v>
-      </c>
       <c r="L5" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="B6" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>65</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="F6" s="17" t="s">
-        <v>251</v>
-      </c>
       <c r="L6" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="C7" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="L7" s="17" t="s">
         <v>253</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="C8" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>83</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
@@ -10290,7 +10287,7 @@
         <v>77</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
@@ -10298,7 +10295,7 @@
         <v>85</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
@@ -10306,15 +10303,15 @@
         <v>90</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="C12" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>260</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
@@ -10322,7 +10319,7 @@
         <v>101</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
@@ -10330,7 +10327,7 @@
         <v>107</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
@@ -10338,36 +10335,36 @@
         <v>113</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="C16" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>265</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="17" spans="3:4" ht="15" customHeight="1">
       <c r="C17" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>267</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="18" spans="3:4" ht="15" customHeight="1">
       <c r="C18" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>269</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="19" spans="3:4" ht="15" customHeight="1">
       <c r="C19" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>162</v>
@@ -10375,50 +10372,50 @@
     </row>
     <row r="20" spans="3:4" ht="15" customHeight="1">
       <c r="C20" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>272</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="21" spans="3:4" ht="15" customHeight="1">
       <c r="C21" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>274</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15" customHeight="1">
       <c r="C22" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>276</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15" customHeight="1">
       <c r="C23" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" s="17" t="s">
         <v>278</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="24" spans="3:4" ht="15" customHeight="1">
       <c r="C24" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>280</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="25" spans="3:4" ht="15" customHeight="1">
       <c r="C25" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>282</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="26" spans="3:4" ht="15" customHeight="1">
@@ -10426,17 +10423,17 @@
         <v>164</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27" spans="3:4" ht="15" customHeight="1">
       <c r="D27" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28" spans="3:4" ht="15" customHeight="1">
       <c r="C28" s="16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>57</v>
@@ -10444,102 +10441,102 @@
     </row>
     <row r="29" spans="3:4" ht="15" customHeight="1">
       <c r="D29" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="15" customHeight="1">
       <c r="D30" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="3:4" ht="15" customHeight="1">
       <c r="D31" s="17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32" spans="3:4" ht="15" customHeight="1">
       <c r="D32" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="4:4" ht="15" customHeight="1">
       <c r="D33" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="4:4" ht="15" customHeight="1">
       <c r="D34" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="4:4" ht="15" customHeight="1">
       <c r="D35" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="4:4" ht="15" customHeight="1">
       <c r="D36" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37" spans="4:4" ht="15.75" customHeight="1">
       <c r="D37" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="4:4" ht="15.75" customHeight="1">
       <c r="D38" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39" spans="4:4" ht="15.75" customHeight="1">
       <c r="D39" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="4:4" ht="15.75" customHeight="1">
       <c r="D40" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41" spans="4:4" ht="15.75" customHeight="1">
       <c r="D41" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="4:4" ht="15.75" customHeight="1">
       <c r="D42" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43" spans="4:4" ht="15.75" customHeight="1">
       <c r="D43" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="4:4" ht="15.75" customHeight="1">
       <c r="D44" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45" spans="4:4" ht="15.75" customHeight="1">
       <c r="D45" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="4:4" ht="15.75" customHeight="1">
       <c r="D46" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="4:4" ht="15.75" customHeight="1">
       <c r="D47" s="17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48" spans="4:4" ht="15.75" customHeight="1">
       <c r="D48" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1">
@@ -10549,62 +10546,62 @@
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1">
       <c r="D50" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1">
       <c r="D51" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1">
       <c r="D52" s="17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1">
       <c r="D53" s="17" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1">
       <c r="D54" s="17" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1">
       <c r="D55" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1">
       <c r="D56" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1">
       <c r="D57" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1">
       <c r="D58" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1">
       <c r="D59" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="60" spans="4:4" ht="15.75" customHeight="1">
       <c r="D60" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="61" spans="4:4" ht="15.75" customHeight="1">
       <c r="D61" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="62" spans="4:4" ht="15.75" customHeight="1"/>
@@ -11569,12 +11566,12 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1">
       <c r="A1" s="47" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1">
       <c r="A2" s="51" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1">
@@ -11589,21 +11586,21 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1">
       <c r="A5" s="51" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1">
       <c r="A7" s="47"/>
       <c r="B7" s="47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C7" s="47"/>
       <c r="D7" s="47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G7" s="47"/>
       <c r="H7" s="47"/>
@@ -11628,7 +11625,7 @@
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1">
       <c r="A8" s="17" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B8" s="52"/>
       <c r="C8" s="53"/>
@@ -11639,7 +11636,7 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
       <c r="A9" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="53"/>
@@ -11650,7 +11647,7 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" s="17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B10" s="53"/>
       <c r="C10" s="52">
@@ -11670,7 +11667,7 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="53"/>
@@ -11681,7 +11678,7 @@
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="53"/>
@@ -11692,7 +11689,7 @@
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1">
       <c r="A13" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B13" s="53"/>
       <c r="C13" s="52">
@@ -11712,7 +11709,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B14" s="52"/>
       <c r="C14" s="53"/>
@@ -11723,7 +11720,7 @@
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1">
       <c r="A15" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B15" s="52"/>
       <c r="C15" s="53"/>
@@ -11734,7 +11731,7 @@
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1">
       <c r="A16" s="17" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B16" s="53"/>
       <c r="C16" s="52">
@@ -11754,7 +11751,7 @@
     </row>
     <row r="17" spans="1:26" ht="15" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B17" s="52"/>
       <c r="C17" s="53"/>
@@ -11765,7 +11762,7 @@
     </row>
     <row r="18" spans="1:26" ht="15" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B18" s="52"/>
       <c r="C18" s="53"/>
@@ -11776,7 +11773,7 @@
     </row>
     <row r="19" spans="1:26" ht="15" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B19" s="53"/>
       <c r="C19" s="52">
@@ -11796,7 +11793,7 @@
     </row>
     <row r="20" spans="1:26" ht="15" customHeight="1">
       <c r="A20" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="53"/>
@@ -11807,7 +11804,7 @@
     </row>
     <row r="21" spans="1:26" ht="15" customHeight="1">
       <c r="A21" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B21" s="52"/>
       <c r="C21" s="53"/>
@@ -11818,7 +11815,7 @@
     </row>
     <row r="22" spans="1:26" ht="15" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B22" s="53"/>
       <c r="C22" s="52">
@@ -11838,7 +11835,7 @@
     </row>
     <row r="23" spans="1:26" ht="15" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B23" s="53"/>
       <c r="C23" s="52"/>
@@ -11849,7 +11846,7 @@
     </row>
     <row r="24" spans="1:26" ht="15" customHeight="1">
       <c r="A24" s="47" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B24" s="54"/>
       <c r="C24" s="54">
@@ -12875,7 +12872,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
@@ -13986,7 +13983,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>22</v>
@@ -14002,7 +13999,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>25</v>
@@ -14018,7 +14015,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>28</v>
@@ -14034,7 +14031,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>31</v>
@@ -20047,9 +20044,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AY1000"/>
+  <dimension ref="A1:AY999"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -20368,77 +20367,28 @@
       </c>
     </row>
     <row r="4" spans="1:51" ht="12.75" customHeight="1">
-      <c r="A4" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="21">
-        <v>27620</v>
-      </c>
-      <c r="F4" s="22">
-        <v>43941.478217592594</v>
-      </c>
-      <c r="G4" s="22">
-        <v>43941.478217592594</v>
-      </c>
-      <c r="H4" s="23">
-        <v>44012</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="N4" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="R4" s="11">
-        <v>75</v>
-      </c>
-      <c r="S4" s="21">
-        <v>27620</v>
-      </c>
-      <c r="T4" s="22">
-        <v>43941.478217592594</v>
-      </c>
-      <c r="U4" s="24">
-        <v>44012</v>
-      </c>
-      <c r="V4" s="25">
-        <v>113810</v>
-      </c>
-      <c r="W4" s="26">
-        <v>100000</v>
-      </c>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
       <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="27">
-        <v>13810</v>
-      </c>
+      <c r="AD4" s="11"/>
       <c r="AE4" s="11"/>
     </row>
     <row r="5" spans="1:51" ht="12.75" customHeight="1">
@@ -20642,24 +20592,6 @@
       <c r="AE12" s="11"/>
     </row>
     <row r="13" spans="1:51" ht="12.75" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
       <c r="X13" s="11"/>
       <c r="Z13" s="11"/>
       <c r="AB13" s="11"/>
@@ -22108,13 +22040,7 @@
       <c r="AD219" s="11"/>
       <c r="AE219" s="11"/>
     </row>
-    <row r="220" spans="24:31" ht="12.75" customHeight="1">
-      <c r="X220" s="11"/>
-      <c r="Z220" s="11"/>
-      <c r="AB220" s="11"/>
-      <c r="AD220" s="11"/>
-      <c r="AE220" s="11"/>
-    </row>
+    <row r="220" spans="24:31" ht="15.75" customHeight="1"/>
     <row r="221" spans="24:31" ht="15.75" customHeight="1"/>
     <row r="222" spans="24:31" ht="15.75" customHeight="1"/>
     <row r="223" spans="24:31" ht="15.75" customHeight="1"/>
@@ -22894,7 +22820,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="A1:AY1" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
@@ -22939,16 +22864,16 @@
         <v>115</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>120</v>
@@ -22957,13 +22882,13 @@
         <v>121</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>125</v>
@@ -22975,19 +22900,19 @@
         <v>127</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>129</v>
       </c>
       <c r="Q1" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="R1" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="T1" s="8" t="s">
         <v>131</v>
@@ -23076,7 +23001,7 @@
         <v>1234</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E2" s="21">
         <v>2927600</v>
@@ -23108,7 +23033,7 @@
         <v>51</v>
       </c>
       <c r="R2" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="T2" s="17">
         <v>75</v>
@@ -23120,7 +23045,7 @@
         <v>43969.648842592593</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="X2" s="27">
         <v>585520</v>
@@ -27681,22 +27606,22 @@
         <v>114</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>123</v>
@@ -27705,22 +27630,22 @@
         <v>124</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>127</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N1" s="8" t="s">
         <v>129</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>132</v>
@@ -27729,13 +27654,13 @@
         <v>131</v>
       </c>
       <c r="R1" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>190</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>191</v>
       </c>
       <c r="U1" s="19" t="s">
         <v>136</v>
@@ -27806,7 +27731,7 @@
         <v>67</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D2" s="20">
         <v>50311.8</v>
@@ -27839,7 +27764,7 @@
         <v>51</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P2" s="20">
         <v>50311.8</v>
@@ -27848,7 +27773,7 @@
         <v>75</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC2" s="20">
         <v>50311.8</v>
@@ -27862,7 +27787,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="28">
         <v>50529.599999999999</v>
@@ -27893,7 +27818,7 @@
         <v>51</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P3" s="28">
         <v>50529.599999999999</v>
@@ -27902,7 +27827,7 @@
         <v>75</v>
       </c>
       <c r="T3" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC3" s="28">
         <v>50529.599999999999</v>
@@ -27916,7 +27841,7 @@
         <v>61</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="20">
         <v>50856.3</v>
@@ -27949,7 +27874,7 @@
         <v>51</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P4" s="20">
         <v>50856.3</v>
@@ -27958,7 +27883,7 @@
         <v>75</v>
       </c>
       <c r="T4" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AC4" s="20">
         <v>50856.3</v>
@@ -30208,22 +30133,22 @@
         <v>114</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>131</v>
@@ -30309,7 +30234,7 @@
         <v>103</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D2" s="27">
         <v>32416.32</v>
@@ -30318,10 +30243,10 @@
         <v>43987.643125000002</v>
       </c>
       <c r="F2" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="H2" s="17">
         <v>75</v>
@@ -32709,13 +32634,13 @@
         <v>114</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>206</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>207</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>131</v>

</xml_diff>